<commit_message>
Don't save empty cells to file, even if they have conditional formatting applied
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFIsBlank.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFIsBlank.xlsx
@@ -403,12 +403,6 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="0" t="s"/>
-    </x:row>
-    <x:row r="3" spans="1:1">
-      <x:c r="A3" s="0" t="s"/>
-    </x:row>
     <x:row r="4" spans="1:1">
       <x:c r="A4" s="0" t="s">
         <x:v>1</x:v>

</xml_diff>